<commit_message>
Add Updates to Test Data Files
</commit_message>
<xml_diff>
--- a/GUI_Web/src/test/resources/testDataFiles/mainClassExcel.xlsx
+++ b/GUI_Web/src/test/resources/testDataFiles/mainClassExcel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mosta\git\Selenium_E-Commerce_E2E\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mosta\IdeaProjects\ECommerce-SHAFT2\GUI_Web\src\test\resources\testDataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19761A4C-E925-4C0D-AD92-0ECB5FD44D6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864B34D9-F796-4FB7-91C8-8E38E33806F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -184,10 +184,10 @@
     <t>Login6</t>
   </si>
   <si>
-    <t>Mostafanageebelsayed@hotmail.com</t>
-  </si>
-  <si>
     <t>Mostafaahmed9@hotmail.com</t>
+  </si>
+  <si>
+    <t>Mostafanageebelsayed221134567@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -520,13 +520,13 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="35.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
@@ -654,7 +654,7 @@
         <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -662,7 +662,7 @@
         <v>34</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
@@ -712,7 +712,7 @@
         <v>35</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -930,7 +930,7 @@
         <v>49</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -938,7 +938,7 @@
         <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
@@ -988,7 +988,7 @@
         <v>51</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>18</v>
@@ -1005,10 +1005,10 @@
     <hyperlink ref="B8" r:id="rId7" xr:uid="{36489888-78B0-494A-A3CD-B2DF433D0043}"/>
     <hyperlink ref="B9:B10" r:id="rId8" display="Mostafaabcd2020@hotmail.com" xr:uid="{D03A645E-3982-480D-AA15-33B41B1F8B75}"/>
     <hyperlink ref="B12:B13" r:id="rId9" display="Mostafaabcde2021@hotmail.com" xr:uid="{C91020D9-501C-48DA-A0EC-1A40A5EAE8D4}"/>
-    <hyperlink ref="B18:B19" r:id="rId10" display="Mostafanageeb@hotmail.com" xr:uid="{E6F441C9-2493-406B-A0B2-7BD55904A7B4}"/>
-    <hyperlink ref="B19" r:id="rId11" xr:uid="{B3B7D0CD-1CD3-4184-BA2E-FD4890563FB6}"/>
-    <hyperlink ref="B17:B18" r:id="rId12" display="Mostafanageeb@hotmail.com" xr:uid="{6AEC6EE4-A0D8-4B5E-BAB5-1AB933C601BB}"/>
-    <hyperlink ref="B6:B7" r:id="rId13" display="Mostafaahmed9@hotmail.com" xr:uid="{7F995A88-BEF2-4CBE-8B4A-18181680E1B3}"/>
+    <hyperlink ref="B17:B18" r:id="rId10" display="Mostafanageeb@hotmail.com" xr:uid="{6AEC6EE4-A0D8-4B5E-BAB5-1AB933C601BB}"/>
+    <hyperlink ref="B6:B7" r:id="rId11" display="Mostafaahmed9@hotmail.com" xr:uid="{7F995A88-BEF2-4CBE-8B4A-18181680E1B3}"/>
+    <hyperlink ref="B17" r:id="rId12" xr:uid="{4AE62F18-F94C-4AB0-8A56-DD8A5DCEC310}"/>
+    <hyperlink ref="B18:B19" r:id="rId13" display="Mostafanageeb@hotmail.com" xr:uid="{D2BA2BCD-3C06-4574-98F2-B80CC9C7AB2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>

</xml_diff>